<commit_message>
! xong sản phẩm tuần 6 -_-
</commit_message>
<xml_diff>
--- a/6th Week/SE18_DatabaseDesign_v2.0.xlsx
+++ b/6th Week/SE18_DatabaseDesign_v2.0.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="64">
   <si>
     <t>Maxlength</t>
     <phoneticPr fontId="0"/>
@@ -206,6 +206,15 @@
   </si>
   <si>
     <t>UserRole = {Admin, Staff}</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>PhoneNum</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1222,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1223,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,7 +1608,7 @@
         <v>17</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K5" t="s">
         <v>60</v>
@@ -1613,10 +1622,10 @@
         <v>46</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>42</v>
+        <v>63</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -1630,7 +1639,7 @@
         <v>31</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -1646,8 +1655,8 @@
       <c r="G8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>44</v>
+      <c r="I8" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -1822,6 +1831,11 @@
         <v>19</v>
       </c>
     </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
@@ -2285,7 +2299,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>51</v>
@@ -2414,6 +2428,14 @@
         <v>50</v>
       </c>
       <c r="D56" s="3"/>
+      <c r="F56" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
       <c r="K56" s="5" t="s">
         <v>19</v>
       </c>
@@ -2432,6 +2454,14 @@
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
+      <c r="K57" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">

</xml_diff>